<commit_message>
sales upload new templates
</commit_message>
<xml_diff>
--- a/public/templates/sales-upload-template.xlsx
+++ b/public/templates/sales-upload-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6955D0BC-3BFD-4AC9-A1A1-D5A475D99813}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3628A922-65DF-4B53-A6AD-4F2B9F03F37F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,30 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Posted Sales Invoice Lines</t>
-  </si>
-  <si>
-    <t>Posting Date</t>
-  </si>
-  <si>
-    <t>Document No.</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Location Code</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Description 2</t>
-  </si>
-  <si>
-    <t>Item Category Code</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+  <si>
+    <t>Customer List</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>Customer Code</t>
+  </si>
+  <si>
+    <t>Salesman Code</t>
+  </si>
+  <si>
+    <t>Document No./Invoice Number/CM Number</t>
+  </si>
+  <si>
+    <t>Warehouse Code</t>
+  </si>
+  <si>
+    <t>BEVI Sku Code</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -64,10 +61,10 @@
     <t>Line Discount %</t>
   </si>
   <si>
-    <t>06/01/23</t>
-  </si>
-  <si>
-    <t>Item</t>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>PSI-0122311</t>
   </si>
   <si>
     <t>MAIN</t>
@@ -76,47 +73,17 @@
     <t>KS01027</t>
   </si>
   <si>
-    <t>KOJIE SL CLASSIC SOAP 45gx144</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>CAS</t>
-  </si>
-  <si>
-    <t>3,240.00</t>
-  </si>
-  <si>
-    <t>5,496.43</t>
-  </si>
-  <si>
-    <t>6,156.00</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Customer Code</t>
-  </si>
-  <si>
-    <t>Sku Code</t>
-  </si>
-  <si>
-    <t>PSI-010001</t>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>KS01028</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,7 +100,21 @@
     <font>
       <b/>
       <sz val="8"/>
+      <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -151,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,16 +140,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,131 +446,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="16.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>45397</v>
+      </c>
+      <c r="B3" s="4">
+        <v>100001</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3240</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5496.43</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6156</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>45398</v>
+      </c>
+      <c r="B4" s="4">
+        <v>100001</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3">
-        <v>100001</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
+      <c r="I4" s="2">
+        <v>3240</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5496.43</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6156</v>
+      </c>
+      <c r="L4" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>